<commit_message>
fix: Allow Union[str, dict] in validation errors/warnings for Railway compatibility
- Pydantic ValidationResult now accepts both string and dict formats
- Fixes 500 error when Railway returns dict-format validation errors
- Maintains backward compatibility with both formats
</commit_message>
<xml_diff>
--- a/python-api/test_transactions.xlsx
+++ b/python-api/test_transactions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,13 +477,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>125</v>
+        <v>81.45</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>65.16</v>
       </c>
       <c r="D2" t="n">
-        <v>25</v>
+        <v>16.29</v>
       </c>
       <c r="E2" t="n">
         <v>25</v>
@@ -504,24 +504,24 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>250</v>
+        <v>233.65</v>
       </c>
       <c r="C3" t="n">
-        <v>200</v>
+        <v>233.65</v>
       </c>
       <c r="D3" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Elbilsladdning - Station 2</t>
+          <t>Roaming intäkter - Hubject</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4">
@@ -531,25 +531,23 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>150</v>
+        <v>-507.7</v>
       </c>
       <c r="C4" t="n">
-        <v>150</v>
+        <v>-406.16</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>-101.54</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Roaming intäkter - Hubject</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>30</v>
-      </c>
+          <t>Plattformsavgift - Monta</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -558,48 +556,23 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-50</v>
+        <v>-20.32</v>
       </c>
       <c r="C5" t="n">
-        <v>-40</v>
+        <v>-20.32</v>
       </c>
       <c r="D5" t="n">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Plattformsavgift - Monta</t>
+          <t>Övriga kostnader (momsfri)</t>
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>TX005</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>-25</v>
-      </c>
-      <c r="C6" t="n">
-        <v>-20</v>
-      </c>
-      <c r="D6" t="n">
-        <v>-5</v>
-      </c>
-      <c r="E6" t="n">
-        <v>25</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Abonnemangskostnad</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>